<commit_message>
some changes in code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ICGMS Test Data.xlsx
+++ b/src/test/resources/TestData/ICGMS Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\git\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCAA58D3-75B3-4273-881C-E0014543F410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6658FDB3-DACC-4B36-A812-45271B3D2C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SuperAdmin" sheetId="1" r:id="rId1"/>
@@ -31,8 +31,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -109,10 +107,24 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -156,10 +168,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -171,8 +184,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -453,7 +468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -519,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D733CEA-9647-447A-98D3-6257770575AA}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -539,7 +554,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -547,19 +562,19 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1"/>
     </row>
@@ -570,7 +585,7 @@
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="1"/>
@@ -635,10 +650,13 @@
       <c r="B18" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A12" r:id="rId1" xr:uid="{DEEF867C-8DB4-41BC-94AF-66BAC8A4E590}"/>
+    <hyperlink ref="A7" r:id="rId2" xr:uid="{23E87886-9A4E-465F-B032-524B61CDE9BA}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{EA0B2DD6-7380-4BBD-BF0E-EC103FA7DFE8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add updated dropdown for test data
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ICGMS Test Data.xlsx
+++ b/src/test/resources/TestData/ICGMS Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\git\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6658FDB3-DACC-4B36-A812-45271B3D2C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B7CBAD-BE38-4C0E-965B-BD94DB610A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Admin123</t>
   </si>
@@ -107,18 +107,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -168,11 +160,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -184,10 +175,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -532,10 +521,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D733CEA-9647-447A-98D3-6257770575AA}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,7 +533,7 @@
     <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -552,92 +541,93 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>
@@ -649,14 +639,32 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
     </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="A12" r:id="rId1" xr:uid="{DEEF867C-8DB4-41BC-94AF-66BAC8A4E590}"/>
-    <hyperlink ref="A7" r:id="rId2" xr:uid="{23E87886-9A4E-465F-B032-524B61CDE9BA}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{EA0B2DD6-7380-4BBD-BF0E-EC103FA7DFE8}"/>
-  </hyperlinks>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3" xr:uid="{EC3D4E8B-5EE7-4530-A02C-F79C51058DD6}">
+      <formula1>$A$3:$A$15</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{658D99D1-D880-4751-9E70-F12161FD33DC}">
+      <formula1>$A$3:$A$21</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{910D982D-090A-497B-B584-BD7E0865ABD9}">
+      <formula1>$A$3:$A$21</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add dropdown in excel data sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ICGMS Test Data.xlsx
+++ b/src/test/resources/TestData/ICGMS Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\git\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B7CBAD-BE38-4C0E-965B-BD94DB610A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF15A063-B575-4E56-A9C5-1993BEC94860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Customer" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="A0">SuperAdmin!$B$1</definedName>
+    <definedName name="A0">SuperAdmin!$A$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Admin123</t>
   </si>
@@ -46,9 +46,6 @@
     <t>superadmnphase1@owleyes.ch</t>
   </si>
   <si>
-    <t>USERNAME (0,0)</t>
-  </si>
-  <si>
     <t>PASSWORD (0,1)</t>
   </si>
   <si>
@@ -94,20 +91,17 @@
     <t>chandini.khan@sharajman.com</t>
   </si>
   <si>
-    <t>Variable(0,0)</t>
-  </si>
-  <si>
-    <t>USERNAME (0,1)</t>
-  </si>
-  <si>
-    <t>PASSWORD (0,2)</t>
+    <t>SUPERADMIN USERNAME (0,0)</t>
+  </si>
+  <si>
+    <t>CUSTOMER USERNAME (0,0)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,8 +115,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,7 +133,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -163,17 +171,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -455,66 +466,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.109375" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
     <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{C9C1EE53-21AF-47BA-A49C-5638B34CFF63}">
+      <formula1>$A$3:$A$10</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -524,106 +546,106 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.109375" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1"/>
     </row>

</xml_diff>

<commit_message>
output excel uat fields updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ICGMS Test Data.xlsx
+++ b/src/test/resources/TestData/ICGMS Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\git\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF15A063-B575-4E56-A9C5-1993BEC94860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450A6242-5A8B-457C-A3C3-64A561BE0184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SuperAdmin" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Admin123</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>CUSTOMER USERNAME (0,0)</t>
+  </si>
+  <si>
+    <t>judecisla@gmail.com</t>
+  </si>
+  <si>
+    <t>Hello@1234</t>
   </si>
 </sst>
 </file>
@@ -171,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -186,6 +192,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,7 +496,7 @@
     </row>
     <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -499,16 +506,22 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -532,9 +545,12 @@
       <c r="B10" s="1"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{C9C1EE53-21AF-47BA-A49C-5638B34CFF63}">
       <formula1>$A$3:$A$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{A6FBC5BC-3B43-44BF-98CE-562413F2763C}">
+      <formula1>$B$3:$B$10</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -545,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D733CEA-9647-447A-98D3-6257770575AA}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,7 +581,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
excel file repairer added
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ICGMS Test Data.xlsx
+++ b/src/test/resources/TestData/ICGMS Test Data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\git\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450A6242-5A8B-457C-A3C3-64A561BE0184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058F5F43-244D-4791-87D8-41E0CFBFD143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SuperAdmin" sheetId="1" r:id="rId1"/>
     <sheet name="Customer" sheetId="2" r:id="rId2"/>
+    <sheet name="Repairer" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="A0">SuperAdmin!$A$1</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>Admin123</t>
   </si>
@@ -101,6 +102,15 @@
   </si>
   <si>
     <t>Hello@1234</t>
+  </si>
+  <si>
+    <t>REPAIRER USERNAME (0,0)</t>
+  </si>
+  <si>
+    <t>repairerphase1@hamham.uk</t>
+  </si>
+  <si>
+    <t>ehtasham@repairer.com</t>
   </si>
 </sst>
 </file>
@@ -177,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -192,7 +202,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,7 +523,7 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -562,7 +571,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -705,4 +714,85 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{450F6CC7-1659-4DFD-83EC-CFC4B11FFDB1}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" activeCellId="1" sqref="A2 E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="46.109375" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{2D08C1CE-8B77-4399-AE61-B37DE842DDBE}">
+      <formula1>$B$3:$B$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{BC8FA23B-076C-4C85-AA74-2D83E1AD4459}">
+      <formula1>$A$3:$A$10</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
minor changes in pre login
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ICGMS Test Data.xlsx
+++ b/src/test/resources/TestData/ICGMS Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\git\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058F5F43-244D-4791-87D8-41E0CFBFD143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82EF107-2A2F-4480-9595-9BDBD23DBA73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SuperAdmin" sheetId="1" r:id="rId1"/>
@@ -484,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -505,7 +505,7 @@
     </row>
     <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -571,7 +571,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:B21"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -720,7 +720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{450F6CC7-1659-4DFD-83EC-CFC4B11FFDB1}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" activeCellId="1" sqref="A2 E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added insurer in excel data file
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ICGMS Test Data.xlsx
+++ b/src/test/resources/TestData/ICGMS Test Data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\git\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA80FFC-01B5-4E8B-846F-7A2248622E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6817C0-85E7-4641-A920-3B9F297744F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SuperAdmin" sheetId="1" r:id="rId1"/>
     <sheet name="Customer" sheetId="2" r:id="rId2"/>
     <sheet name="Repairer" sheetId="3" r:id="rId3"/>
+    <sheet name="MotorClaim_Insurer" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="A0">SuperAdmin!$A$1</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Admin123</t>
   </si>
@@ -111,6 +112,51 @@
   </si>
   <si>
     <t>ehtasham@repairer.com</t>
+  </si>
+  <si>
+    <t>The Oriental Insurance Company Limited</t>
+  </si>
+  <si>
+    <t>IFFCO TOKIO</t>
+  </si>
+  <si>
+    <t>Chola MS General Insurance</t>
+  </si>
+  <si>
+    <t>Bajaj Allianze General Insurance Co Ltd</t>
+  </si>
+  <si>
+    <t>KOTAK MAHINDRA</t>
+  </si>
+  <si>
+    <t>NATIONAL INSURANCE HI</t>
+  </si>
+  <si>
+    <t>UNITED INDIA</t>
+  </si>
+  <si>
+    <t>TATA AIG</t>
+  </si>
+  <si>
+    <t>Universal Sampo General Insurance</t>
+  </si>
+  <si>
+    <t>MAGMA HDI</t>
+  </si>
+  <si>
+    <t>Royal Sundaram</t>
+  </si>
+  <si>
+    <t>SBI GENERAL</t>
+  </si>
+  <si>
+    <t>THE NEW INDIA ASSURANCE COMPANY LIMITED</t>
+  </si>
+  <si>
+    <t>FGI MOTOR</t>
+  </si>
+  <si>
+    <t>MOTOR CLAIM NAME (0,0)</t>
   </si>
 </sst>
 </file>
@@ -160,7 +206,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -183,11 +229,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -202,6 +257,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D733CEA-9647-447A-98D3-6257770575AA}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -721,7 +778,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" activeCellId="1" sqref="A2 E6"/>
+      <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -795,4 +852,130 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{406AC4F8-FC07-4DBB-8B8D-E8F510D8C3D7}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="46.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A16">
+    <sortCondition ref="A16"/>
+  </sortState>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{D2C4C77C-FFB2-4AE5-9C68-B26D64C3DDC7}">
+      <formula1>$A$3:$A$21</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{453B8315-715A-4C12-B8E8-D61B9B8CDBA3}">
+      <formula1>$A$3:$A$21</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
few function of color added
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ICGMS Test Data.xlsx
+++ b/src/test/resources/TestData/ICGMS Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\git\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6817C0-85E7-4641-A920-3B9F297744F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FE7890-69EB-43D1-8DC9-6742B4080AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>Admin123</t>
   </si>
@@ -157,6 +157,15 @@
   </si>
   <si>
     <t>MOTOR CLAIM NAME (0,0)</t>
+  </si>
+  <si>
+    <t>ICICI</t>
+  </si>
+  <si>
+    <t>HFDC ERGO</t>
+  </si>
+  <si>
+    <t>LIBERTY</t>
   </si>
 </sst>
 </file>
@@ -628,7 +637,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A21"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -647,7 +656,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -778,7 +787,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -856,7 +865,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{406AC4F8-FC07-4DBB-8B8D-E8F510D8C3D7}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -871,106 +880,143 @@
       <c r="A1" s="5" t="s">
         <v>38</v>
       </c>
+      <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>37</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B2" s="6"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="B3" s="6"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B4" s="6"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="B5" s="6"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>25</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B6" s="6"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B7" s="6"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>29</v>
+      <c r="A9" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B9" s="6"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="B10" s="6"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B11" s="6"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>31</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B12" s="6"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B13" s="6"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B14" s="6"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B15" s="6"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="6"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" s="6"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
+      <c r="B21" s="6"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A16">
-    <sortCondition ref="A16"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A21">
+    <sortCondition ref="A3:A21"/>
   </sortState>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{D2C4C77C-FFB2-4AE5-9C68-B26D64C3DDC7}">
-      <formula1>$A$3:$A$21</formula1>
+      <formula1>$A$3:$A$25</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{453B8315-715A-4C12-B8E8-D61B9B8CDBA3}">
       <formula1>$A$3:$A$21</formula1>

</xml_diff>

<commit_message>
updated script 1 and 2 motor claim
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ICGMS Test Data.xlsx
+++ b/src/test/resources/TestData/ICGMS Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\git\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D948262-9127-4AB6-8935-19F6C7EDA84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2A9D93-DF50-4089-BFBE-9C4129ECCA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>Admin123</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>custphase1@catgroup.uk</t>
+  </si>
+  <si>
+    <t>zooowlwhy@quicksend.ch</t>
+  </si>
+  <si>
+    <t>client@client.com</t>
   </si>
 </sst>
 </file>
@@ -218,7 +224,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -263,11 +269,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -284,6 +299,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -577,71 +598,67 @@
     <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>44</v>
+      </c>
       <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{A6FBC5BC-3B43-44BF-98CE-562413F2763C}">
+      <formula1>$B$3:$B$5</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{C9C1EE53-21AF-47BA-A49C-5638B34CFF63}">
-      <formula1>$A$3:$A$10</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{A6FBC5BC-3B43-44BF-98CE-562413F2763C}">
-      <formula1>$B$3:$B$10</formula1>
+      <formula1>$A$3:$A$6</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -650,10 +667,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D733CEA-9647-447A-98D3-6257770575AA}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -697,79 +714,85 @@
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
+      <c r="A6" t="s">
+        <v>43</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>14</v>
-      </c>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="B15" s="1"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B17" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 A2" xr:uid="{EC3D4E8B-5EE7-4530-A02C-F79C51058DD6}">
-      <formula1>$A$3:$A$16</formula1>
+      <formula1>$A$3:$A$17</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{658D99D1-D880-4751-9E70-F12161FD33DC}">
-      <formula1>$A$3:$A$16</formula1>
+      <formula1>$A$3:$A$17</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -779,10 +802,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{450F6CC7-1659-4DFD-83EC-CFC4B11FFDB1}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -821,37 +844,13 @@
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-    </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{2D08C1CE-8B77-4399-AE61-B37DE842DDBE}">
-      <formula1>$B$3:$B$10</formula1>
+      <formula1>$B$3:$B$4</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{BC8FA23B-076C-4C85-AA74-2D83E1AD4459}">
-      <formula1>$A$3:$A$10</formula1>
+      <formula1>$A$3:$A$4</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -860,7 +859,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{406AC4F8-FC07-4DBB-8B8D-E8F510D8C3D7}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -879,7 +878,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B2" s="6"/>
     </row>
@@ -985,36 +984,16 @@
       </c>
       <c r="B19" s="6"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="6"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="6"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A21">
-    <sortCondition ref="A3:A21"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A19">
+    <sortCondition ref="A19"/>
   </sortState>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{D2C4C77C-FFB2-4AE5-9C68-B26D64C3DDC7}">
-      <formula1>$A$3:$A$25</formula1>
+      <formula1>$A$3:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{453B8315-715A-4C12-B8E8-D61B9B8CDBA3}">
-      <formula1>$A$3:$A$21</formula1>
+      <formula1>$A$3:$A$19</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new 8th step added
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ICGMS Test Data.xlsx
+++ b/src/test/resources/TestData/ICGMS Test Data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\git\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2A9D93-DF50-4089-BFBE-9C4129ECCA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21824739-1296-439A-AF97-14ED6ACEAA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SuperAdmin" sheetId="1" r:id="rId1"/>
-    <sheet name="Customer" sheetId="2" r:id="rId2"/>
-    <sheet name="Repairer" sheetId="3" r:id="rId3"/>
-    <sheet name="MotorClaim_Insurer" sheetId="4" r:id="rId4"/>
+    <sheet name="MotorClaim_Insurer" sheetId="4" r:id="rId1"/>
+    <sheet name="SuperAdmin" sheetId="1" r:id="rId2"/>
+    <sheet name="Customer" sheetId="2" r:id="rId3"/>
+    <sheet name="Repairer" sheetId="3" r:id="rId4"/>
+    <sheet name="Insurer_Log" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="A0">SuperAdmin!$A$1</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>Admin123</t>
   </si>
@@ -175,6 +176,12 @@
   </si>
   <si>
     <t>client@client.com</t>
+  </si>
+  <si>
+    <t>INSURER USERNAME (0,0)</t>
+  </si>
+  <si>
+    <t>royalsundaram@insurer.com</t>
   </si>
 </sst>
 </file>
@@ -302,9 +309,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,6 +593,149 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{406AC4F8-FC07-4DBB-8B8D-E8F510D8C3D7}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="46.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="6"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="6"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="6"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="6"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="6"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="6"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="6"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A19">
+    <sortCondition ref="A19"/>
+  </sortState>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{D2C4C77C-FFB2-4AE5-9C68-B26D64C3DDC7}">
+      <formula1>$A$3:$A$19</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{453B8315-715A-4C12-B8E8-D61B9B8CDBA3}">
+      <formula1>$A$3:$A$19</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -626,10 +778,10 @@
       <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="6"/>
@@ -642,15 +794,15 @@
       <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -665,7 +817,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D733CEA-9647-447A-98D3-6257770575AA}">
   <dimension ref="A1:B17"/>
   <sheetViews>
@@ -800,12 +952,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{450F6CC7-1659-4DFD-83EC-CFC4B11FFDB1}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -857,143 +1009,55 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{406AC4F8-FC07-4DBB-8B8D-E8F510D8C3D7}">
-  <dimension ref="A1:B19"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F5B4E21-4410-419D-84B4-FDBA09D16EC8}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46.109375" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="6"/>
+        <v>45</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="6"/>
+      <c r="A2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="6"/>
+      <c r="A3" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="6"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="6"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="6"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="6"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="6"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="6"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="6"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="6"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="6"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="6"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="6"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="6"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="6"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="6"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="6"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="6"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A19">
-    <sortCondition ref="A19"/>
-  </sortState>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{D2C4C77C-FFB2-4AE5-9C68-B26D64C3DDC7}">
-      <formula1>$A$3:$A$19</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{1EF0B0DD-F69A-4DC4-8236-CE5AB0088706}">
+      <formula1>$A$3:$A$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{453B8315-715A-4C12-B8E8-D61B9B8CDBA3}">
-      <formula1>$A$3:$A$19</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{7621F179-7E40-4883-8A29-82523EE43A2A}">
+      <formula1>$B$3:$B$4</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
13 feb updates and added 3 new steps motor claim
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ICGMS Test Data.xlsx
+++ b/src/test/resources/TestData/ICGMS Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\git\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21824739-1296-439A-AF97-14ED6ACEAA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D49B3A-E561-434E-AE19-508AED1DBFDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MotorClaim_Insurer" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
   <si>
     <t>Admin123</t>
   </si>
@@ -94,9 +94,6 @@
     <t>chandini.khan@sharajman.com</t>
   </si>
   <si>
-    <t>SUPERADMIN USERNAME (0,0)</t>
-  </si>
-  <si>
     <t>CUSTOMER USERNAME (0,0)</t>
   </si>
   <si>
@@ -163,9 +160,6 @@
     <t>ICICI</t>
   </si>
   <si>
-    <t>HFDC ERGO</t>
-  </si>
-  <si>
     <t>LIBERTY</t>
   </si>
   <si>
@@ -182,6 +176,15 @@
   </si>
   <si>
     <t>royalsundaram@insurer.com</t>
+  </si>
+  <si>
+    <t>HDFC ERGO</t>
+  </si>
+  <si>
+    <t>SUPERADMIN AND CLIENT USERNAME (0,0)</t>
+  </si>
+  <si>
+    <t>testclient1@catgroup.uk</t>
   </si>
 </sst>
 </file>
@@ -289,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -313,7 +316,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,7 +599,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,115 +609,115 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B2" s="6"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="6"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="6"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="6"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B6" s="6"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="6"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="6"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B10" s="6"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="6"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="6"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="6"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="6"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="6"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="6"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="6"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="6"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="6"/>
     </row>
@@ -737,22 +739,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.109375" customWidth="1"/>
+    <col min="1" max="1" width="48.33203125" customWidth="1"/>
     <col min="2" max="2" width="26.6640625" customWidth="1"/>
     <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>2</v>
@@ -779,10 +781,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
         <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
       </c>
       <c r="C4" s="6"/>
     </row>
@@ -794,15 +796,22 @@
       <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>44</v>
+      <c r="A6" t="s">
+        <v>47</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -810,7 +819,7 @@
       <formula1>$B$3:$B$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{C9C1EE53-21AF-47BA-A49C-5638B34CFF63}">
-      <formula1>$A$3:$A$6</formula1>
+      <formula1>$A$3:$A$7</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -822,7 +831,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -833,7 +842,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>2</v>
@@ -841,7 +850,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -867,7 +876,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1"/>
     </row>
@@ -897,7 +906,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1"/>
     </row>
@@ -957,7 +966,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -968,7 +977,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>2</v>
@@ -976,7 +985,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -984,7 +993,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -992,7 +1001,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1"/>
     </row>
@@ -1013,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F5B4E21-4410-419D-84B4-FDBA09D16EC8}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1025,7 +1034,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>2</v>
@@ -1033,15 +1042,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
-        <v>46</v>
+      <c r="A3" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
new 13 14 15 16 added and few changes in old
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ICGMS Test Data.xlsx
+++ b/src/test/resources/TestData/ICGMS Test Data.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\git\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D49B3A-E561-434E-AE19-508AED1DBFDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75535312-6004-432C-902A-1F1046B6E630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MotorClaim_Insurer" sheetId="4" r:id="rId1"/>
-    <sheet name="SuperAdmin" sheetId="1" r:id="rId2"/>
-    <sheet name="Customer" sheetId="2" r:id="rId3"/>
-    <sheet name="Repairer" sheetId="3" r:id="rId4"/>
-    <sheet name="Insurer_Log" sheetId="5" r:id="rId5"/>
+    <sheet name="PreInspection_Type" sheetId="7" r:id="rId2"/>
+    <sheet name="SuperAdmin" sheetId="1" r:id="rId3"/>
+    <sheet name="Customer" sheetId="2" r:id="rId4"/>
+    <sheet name="Repairer" sheetId="3" r:id="rId5"/>
+    <sheet name="Surveyor" sheetId="6" r:id="rId6"/>
+    <sheet name="Insurer_Log" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="A0">SuperAdmin!$A$1</definedName>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
   <si>
     <t>Admin123</t>
   </si>
@@ -185,6 +187,33 @@
   </si>
   <si>
     <t>testclient1@catgroup.uk</t>
+  </si>
+  <si>
+    <t>SURVEYOR USERNAME (0,0)</t>
+  </si>
+  <si>
+    <t>surveyorphase1@sendnow.win</t>
+  </si>
+  <si>
+    <t>ehtasham@surveyororg.com</t>
+  </si>
+  <si>
+    <t>PRE INSPECTION TYPE (0,0)</t>
+  </si>
+  <si>
+    <t>Car</t>
+  </si>
+  <si>
+    <t>Commercial vehicles</t>
+  </si>
+  <si>
+    <t>Construction equipment's</t>
+  </si>
+  <si>
+    <t>Miscellaneous equipment's</t>
+  </si>
+  <si>
+    <t>2-wheeler</t>
   </si>
 </sst>
 </file>
@@ -599,7 +628,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection sqref="A1:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -738,11 +767,73 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C328D9B2-1623-4948-9159-E6B4FC032A88}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="46.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{7D659341-99AB-47F3-9F00-3CB3A3055FE2}">
+      <formula1>$A$3:$A$7</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{BBD052BF-1499-4B6F-8288-6599F7E34327}">
+      <formula1>$A$3:$A$7</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -826,12 +917,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D733CEA-9647-447A-98D3-6257770575AA}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -850,7 +941,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -961,12 +1052,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{450F6CC7-1659-4DFD-83EC-CFC4B11FFDB1}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1018,12 +1109,69 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E41ABD4A-1C7D-4BEA-8306-D714B0819D20}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="46.109375" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="1"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{6BEFE3BA-BBEE-4D8D-8D2B-E98E86D98E53}">
+      <formula1>$A$3:$A$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{2552C37B-A202-4580-8249-8E7209909168}">
+      <formula1>$B$3:$B$4</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F5B4E21-4410-419D-84B4-FDBA09D16EC8}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updates in  steps 1 and step 9 of motor claim
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ICGMS Test Data.xlsx
+++ b/src/test/resources/TestData/ICGMS Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\git\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75535312-6004-432C-902A-1F1046B6E630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB59D3A1-52A0-4A3A-A6E0-481EF4FE1B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="719" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MotorClaim_Insurer" sheetId="4" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
   <si>
     <t>Admin123</t>
   </si>
@@ -214,6 +214,15 @@
   </si>
   <si>
     <t>2-wheeler</t>
+  </si>
+  <si>
+    <t>@3KVs1Hx</t>
+  </si>
+  <si>
+    <t>testuatrepairer1@honeys.be</t>
+  </si>
+  <si>
+    <t>testrepairer1@catgroup.uk</t>
   </si>
 </sst>
 </file>
@@ -263,7 +272,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -317,11 +326,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -345,6 +367,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,7 +653,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A19"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -833,7 +858,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C9" activeCellId="1" sqref="A2 C9:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -919,10 +944,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D733CEA-9647-447A-98D3-6257770575AA}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -931,7 +956,7 @@
     <col min="2" max="2" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -939,93 +964,100 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" s="11"/>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1039,12 +1071,15 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 A2" xr:uid="{EC3D4E8B-5EE7-4530-A02C-F79C51058DD6}">
       <formula1>$A$3:$A$17</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{658D99D1-D880-4751-9E70-F12161FD33DC}">
       <formula1>$A$3:$A$17</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{6CA87FD2-14FB-47B1-B41E-D731243E3ACF}">
+      <formula1>$B$3:$B$4</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1054,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{450F6CC7-1659-4DFD-83EC-CFC4B11FFDB1}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1076,7 +1111,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -1091,18 +1126,31 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B6" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{2D08C1CE-8B77-4399-AE61-B37DE842DDBE}">
-      <formula1>$B$3:$B$4</formula1>
+      <formula1>$B$3:$B$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{BC8FA23B-076C-4C85-AA74-2D83E1AD4459}">
-      <formula1>$A$3:$A$4</formula1>
+      <formula1>$A$3:$A$6</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1114,7 +1162,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1171,7 +1219,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
changes Step 5 of Motor claim
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ICGMS Test Data.xlsx
+++ b/src/test/resources/TestData/ICGMS Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\git\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604E0190-46F1-40DD-8AE4-182E24E939F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A073A688-2A2D-4858-85D9-B80A335161A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="719" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="719" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MotorClaim_Insurer" sheetId="4" r:id="rId1"/>
@@ -945,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D733CEA-9647-447A-98D3-6257770575AA}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1090,8 +1090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{450F6CC7-1659-4DFD-83EC-CFC4B11FFDB1}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1110,7 +1110,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
9 step of motor claim corrected and all 18 steps working ok
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ICGMS Test Data.xlsx
+++ b/src/test/resources/TestData/ICGMS Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\git\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A073A688-2A2D-4858-85D9-B80A335161A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C165F2CD-BE2F-4792-967B-53CA9BA04CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="719" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="719" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MotorClaim_Insurer" sheetId="4" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
   <si>
     <t>Admin123</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>testrepairer1@catgroup.uk</t>
+  </si>
+  <si>
+    <t>hataidme@sendapp.uk</t>
   </si>
 </sst>
 </file>
@@ -343,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -369,6 +372,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,7 +656,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -943,10 +947,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D733CEA-9647-447A-98D3-6257770575AA}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -965,7 +969,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -1015,67 +1019,73 @@
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="B12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>14</v>
-      </c>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="B16" s="1"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B18" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 A2" xr:uid="{EC3D4E8B-5EE7-4530-A02C-F79C51058DD6}">
-      <formula1>$A$3:$A$17</formula1>
+      <formula1>$A$3:$A$18</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{658D99D1-D880-4751-9E70-F12161FD33DC}">
-      <formula1>$A$3:$A$17</formula1>
+      <formula1>$A$3:$A$18</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{6CA87FD2-14FB-47B1-B41E-D731243E3ACF}">
       <formula1>$B$3:$B$4</formula1>
@@ -1090,7 +1100,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{450F6CC7-1659-4DFD-83EC-CFC4B11FFDB1}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -1217,8 +1227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F5B4E21-4410-419D-84B4-FDBA09D16EC8}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" activeCellId="1" sqref="F14 B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
motor claim all steps and verified completed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ICGMS Test Data.xlsx
+++ b/src/test/resources/TestData/ICGMS Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\git\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C165F2CD-BE2F-4792-967B-53CA9BA04CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0009B35-CB6A-4711-BC40-9C7FC33CBBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="719" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="719" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MotorClaim_Insurer" sheetId="4" r:id="rId1"/>
@@ -346,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -372,7 +372,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -949,7 +948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D733CEA-9647-447A-98D3-6257770575AA}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -969,7 +968,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -1019,7 +1018,7 @@
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
+      <c r="A9" t="s">
         <v>60</v>
       </c>
       <c r="B9" s="1"/>
@@ -1227,7 +1226,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F5B4E21-4410-419D-84B4-FDBA09D16EC8}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" activeCellId="1" sqref="F14 B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
time sleeps and screenshots added
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ICGMS Test Data.xlsx
+++ b/src/test/resources/TestData/ICGMS Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parth Grover\eclipse-workspace\AutomationICGMS\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAC5905-7A39-455D-9132-C7E6A434BD15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4608656-1656-4C2C-AA03-0E558809060C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="719" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="719" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MotorClaim_Insurer" sheetId="4" r:id="rId1"/>
@@ -228,7 +228,7 @@
     <t>chanchlesh.sharma@sharajman.com</t>
   </si>
   <si>
-    <t>x1@psPr1</t>
+    <t>0Fb@wAc2</t>
   </si>
 </sst>
 </file>
@@ -862,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -952,7 +952,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -971,7 +971,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -1110,7 +1110,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1179,7 +1179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E41ABD4A-1C7D-4BEA-8306-D714B0819D20}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
test data issue update
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ICGMS Test Data.xlsx
+++ b/src/test/resources/TestData/ICGMS Test Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parth Grover\eclipse-workspace\AutomationICGMS\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\git\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4608656-1656-4C2C-AA03-0E558809060C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2157138-799D-4B45-9FAD-CEABA73A71F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="719" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="719" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MotorClaim_Insurer" sheetId="4" r:id="rId1"/>
@@ -228,7 +228,7 @@
     <t>chanchlesh.sharma@sharajman.com</t>
   </si>
   <si>
-    <t>0Fb@wAc2</t>
+    <t>x1@psPr1</t>
   </si>
 </sst>
 </file>
@@ -863,7 +863,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -952,7 +952,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1110,7 +1110,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1179,7 +1179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E41ABD4A-1C7D-4BEA-8306-D714B0819D20}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1236,7 +1236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F5B4E21-4410-419D-84B4-FDBA09D16EC8}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>

</xml_diff>